<commit_message>
Added PROD login and End Date check
</commit_message>
<xml_diff>
--- a/Inputs/Scenarios.xlsx
+++ b/Inputs/Scenarios.xlsx
@@ -1,15 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <x:workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MKR7550\Documents\UiPath\RPA_Exclusion\Inputs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10E187B8-04AF-46F9-8AC0-6E7DE26A6400}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
-    <x:workbookView firstSheet="0" activeTab="0"/>
+    <x:workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Scenarios" sheetId="1" r:id="rId2"/>
+    <x:sheet name="Scenarios" sheetId="1" r:id="rId1"/>
   </x:sheets>
   <x:definedNames/>
-  <x:calcPr calcId="125725"/>
+  <x:calcPr calcId="0"/>
 </x:workbook>
 </file>
 
@@ -43,9 +50,6 @@
     <x:t>Delivery 1</x:t>
   </x:si>
   <x:si>
-    <x:t>All</x:t>
-  </x:si>
-  <x:si>
     <x:t>Menulog</x:t>
   </x:si>
   <x:si>
@@ -128,18 +132,23 @@
   </x:si>
   <x:si>
     <x:t>Dont show Menulog kiosk items</x:t>
+  </x:si>
+  <x:si>
+    <x:t>KFC Morayfield East, KFC Wright</x:t>
+  </x:si>
+  <x:si>
+    <x:t/>
   </x:si>
 </x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<x:styleSheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac x16r2 xr">
   <x:numFmts count="1">
     <x:numFmt numFmtId="0" formatCode=""/>
   </x:numFmts>
-  <x:fonts count="1">
+  <x:fonts count="1" x14ac:knownFonts="1">
     <x:font>
-      <x:vertAlign val="baseline"/>
       <x:sz val="11"/>
       <x:color rgb="FF000000"/>
       <x:name val="Calibri"/>
@@ -155,38 +164,32 @@
     </x:fill>
   </x:fills>
   <x:borders count="1">
-    <x:border diagonalUp="0" diagonalDown="0">
-      <x:left style="none">
-        <x:color rgb="FF000000"/>
-      </x:left>
-      <x:right style="none">
-        <x:color rgb="FF000000"/>
-      </x:right>
-      <x:top style="none">
-        <x:color rgb="FF000000"/>
-      </x:top>
-      <x:bottom style="none">
-        <x:color rgb="FF000000"/>
-      </x:bottom>
-      <x:diagonal style="none">
-        <x:color rgb="FF000000"/>
-      </x:diagonal>
+    <x:border>
+      <x:left/>
+      <x:right/>
+      <x:top/>
+      <x:bottom/>
+      <x:diagonal/>
     </x:border>
   </x:borders>
   <x:cellStyleXfs count="1">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
   </x:cellStyleXfs>
   <x:cellXfs count="1">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </x:cellXfs>
   <x:cellStyles count="1">
     <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
   </x:cellStyles>
+  <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <x:extLst>
+    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </x:ext>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </x:ext>
+  </x:extLst>
 </x:styleSheet>
 </file>
 
@@ -474,17 +477,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
   <x:dimension ref="A1:H9"/>
   <x:sheetViews>
-    <x:sheetView workbookViewId="0"/>
+    <x:sheetView tabSelected="1" workbookViewId="0">
+      <x:selection activeCell="A1" sqref="A1 A1:E1"/>
+    </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:sheetData>
-    <x:row r="1" spans="1:8">
+    <x:row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -510,212 +515,212 @@
         <x:v>7</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:8">
+    <x:row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <x:c r="A2" s="0" t="s">
         <x:v>8</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="C2" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
-      <x:c r="C2" s="0" t="s">
+      <x:c r="D2" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="D2" s="0" t="s">
+      <x:c r="E2" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="E2" s="0" t="s">
+      <x:c r="F2" s="0" t="s">
         <x:v>12</x:v>
       </x:c>
-      <x:c r="F2" s="0" t="s">
+      <x:c r="G2" s="0" t="s">
         <x:v>13</x:v>
       </x:c>
-      <x:c r="G2" s="0" t="s">
+      <x:c r="H2" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <x:c r="A3" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="C3" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D3" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="E3" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F3" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="G3" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="H3" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <x:c r="A4" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="D4" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="E4" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="F4" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="G4" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="H4" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <x:c r="A5" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="C5" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="D5" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="E5" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F5" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="G5" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="H5" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <x:c r="A6" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="B6" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="C6" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="D6" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="E6" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="F6" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="G6" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="H6" s="0" t="s">
         <x:v>14</x:v>
       </x:c>
-      <x:c r="H2" s="0" t="s">
-        <x:v>15</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="3" spans="1:8">
-      <x:c r="A3" s="0" t="s">
+    </x:row>
+    <x:row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <x:c r="A7" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="B7" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="C7" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="D7" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="E7" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="F7" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="G7" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="H7" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <x:c r="A8" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="B8" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="C8" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="D8" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="E8" s="0" t="s">
         <x:v>16</x:v>
       </x:c>
-      <x:c r="B3" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="C3" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="D3" s="0" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="E3" s="0" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="F3" s="0" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="G3" s="0" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="H3" s="0" t="s">
-        <x:v>15</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:8">
-      <x:c r="A4" s="0" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="B4" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="C4" s="0" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="D4" s="0" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="E4" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="F4" s="0" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="G4" s="0" t="s">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="H4" s="0" t="s">
-        <x:v>15</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:8">
-      <x:c r="A5" s="0" t="s">
+      <x:c r="F8" s="0" t="s">
         <x:v>24</x:v>
       </x:c>
-      <x:c r="B5" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="C5" s="0" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="D5" s="0" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="E5" s="0" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="F5" s="0" t="s">
-        <x:v>25</x:v>
-      </x:c>
-      <x:c r="G5" s="0" t="s">
-        <x:v>26</x:v>
-      </x:c>
-      <x:c r="H5" s="0" t="s">
-        <x:v>15</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="6" spans="1:8">
-      <x:c r="A6" s="0" t="s">
-        <x:v>27</x:v>
-      </x:c>
-      <x:c r="B6" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="C6" s="0" t="s">
+      <x:c r="G8" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="H8" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <x:c r="A9" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="B9" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="C9" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="D9" s="0" t="s">
         <x:v>28</x:v>
       </x:c>
-      <x:c r="D6" s="0" t="s">
-        <x:v>29</x:v>
-      </x:c>
-      <x:c r="E6" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="F6" s="0" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="G6" s="0" t="s">
-        <x:v>30</x:v>
-      </x:c>
-      <x:c r="H6" s="0" t="s">
-        <x:v>15</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="7" spans="1:8">
-      <x:c r="A7" s="0" t="s">
-        <x:v>31</x:v>
-      </x:c>
-      <x:c r="B7" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="C7" s="0" t="s">
-        <x:v>32</x:v>
-      </x:c>
-      <x:c r="D7" s="0" t="s">
-        <x:v>29</x:v>
-      </x:c>
-      <x:c r="E7" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="F7" s="0" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="G7" s="0" t="s">
-        <x:v>33</x:v>
-      </x:c>
-      <x:c r="H7" s="0" t="s">
-        <x:v>15</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="8" spans="1:8">
-      <x:c r="A8" s="0" t="s">
-        <x:v>34</x:v>
-      </x:c>
-      <x:c r="B8" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="C8" s="0" t="s">
-        <x:v>28</x:v>
-      </x:c>
-      <x:c r="D8" s="0" t="s">
-        <x:v>29</x:v>
-      </x:c>
-      <x:c r="E8" s="0" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="F8" s="0" t="s">
-        <x:v>25</x:v>
-      </x:c>
-      <x:c r="G8" s="0" t="s">
-        <x:v>35</x:v>
-      </x:c>
-      <x:c r="H8" s="0" t="s">
-        <x:v>15</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="9" spans="1:8">
-      <x:c r="A9" s="0" t="s">
+      <x:c r="E9" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F9" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="G9" s="0" t="s">
         <x:v>36</x:v>
       </x:c>
-      <x:c r="B9" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="C9" s="0" t="s">
-        <x:v>32</x:v>
-      </x:c>
-      <x:c r="D9" s="0" t="s">
-        <x:v>29</x:v>
-      </x:c>
-      <x:c r="E9" s="0" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="F9" s="0" t="s">
-        <x:v>25</x:v>
-      </x:c>
-      <x:c r="G9" s="0" t="s">
-        <x:v>37</x:v>
-      </x:c>
       <x:c r="H9" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>14</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>